<commit_message>
redaction test fonctionnel + peluchage
</commit_message>
<xml_diff>
--- a/chess_tournament/unittest/structure_data_test.xlsx
+++ b/chess_tournament/unittest/structure_data_test.xlsx
@@ -1,23 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnc\Documents\projets\039 - formation OC\04-projet4-TournoisEchec\chess_tournament\chess_tournament\unittest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B127ECEF-DF9C-438E-9D87-AF47828BBCB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{301D7DCE-0A25-4C1F-8FC4-2985FA245680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28785" yWindow="-15870" windowWidth="16440" windowHeight="29040" xr2:uid="{1B949F2A-8B06-44D6-8BEB-6702FE846320}"/>
+    <workbookView xWindow="3228" yWindow="1452" windowWidth="16380" windowHeight="8808" activeTab="3" xr2:uid="{1B949F2A-8B06-44D6-8BEB-6702FE846320}"/>
   </bookViews>
   <sheets>
     <sheet name="match" sheetId="1" r:id="rId1"/>
     <sheet name="score" sheetId="2" r:id="rId2"/>
+    <sheet name="match_fct" sheetId="3" r:id="rId3"/>
+    <sheet name="score_fct" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">match!$A$1:$H$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">match_fct!$A$1:$H$17</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="61">
   <si>
     <t>joueur</t>
   </si>
@@ -172,6 +175,54 @@
   </si>
   <si>
     <t>joueur_1</t>
+  </si>
+  <si>
+    <t>tour1_class</t>
+  </si>
+  <si>
+    <t>tour1_score</t>
+  </si>
+  <si>
+    <t>tour1_tot</t>
+  </si>
+  <si>
+    <t>tour2_class</t>
+  </si>
+  <si>
+    <t>tour2_score</t>
+  </si>
+  <si>
+    <t>tour2_tot</t>
+  </si>
+  <si>
+    <t>tour3_class</t>
+  </si>
+  <si>
+    <t>tour3_score</t>
+  </si>
+  <si>
+    <t>tour3_tot</t>
+  </si>
+  <si>
+    <t>tour4_class</t>
+  </si>
+  <si>
+    <t>tour4_score</t>
+  </si>
+  <si>
+    <t>tour4_tot</t>
+  </si>
+  <si>
+    <t>rang</t>
+  </si>
+  <si>
+    <t>round_2</t>
+  </si>
+  <si>
+    <t>match_5</t>
+  </si>
+  <si>
+    <t>match_6</t>
   </si>
 </sst>
 </file>
@@ -209,7 +260,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -217,11 +268,180 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -230,11 +450,61 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="20">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -281,6 +551,28 @@
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -295,17 +587,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F161EF05-900C-4F45-9463-1F75D7ABD29C}" name="Tableau1" displayName="Tableau1" ref="A1:H17" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F161EF05-900C-4F45-9463-1F75D7ABD29C}" name="Tableau1" displayName="Tableau1" ref="A1:H17" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="A1:H17" xr:uid="{1FEF8CB5-F46E-43DE-981B-DE10EB7B0593}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{76DA34E3-67C7-488D-A86C-2BD6C78D2F4A}" name="tour" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{FB5D22A2-7FFE-4B5D-B773-A70868A20EE9}" name="match" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{80BD9112-B795-4FC0-84B3-EF21AFEF203A}" name="joueur_1" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{41BF02E4-59D4-4006-AF96-C05B0D0EEA22}" name="couleur_1" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{1D1B1DBE-DA05-46F4-BA65-257985C82CB9}" name="score_1" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{C0BE1A05-5129-40A8-86C3-5B5052FF93BC}" name="score_2" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{859D60A2-6C69-45D2-8EF3-A58DF97DBC38}" name="couleur_2" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{2D02D19C-6174-4ACC-9EE3-74CAE6D8C11F}" name="joueur_2" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{76DA34E3-67C7-488D-A86C-2BD6C78D2F4A}" name="tour" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{FB5D22A2-7FFE-4B5D-B773-A70868A20EE9}" name="match" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{80BD9112-B795-4FC0-84B3-EF21AFEF203A}" name="joueur_1" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{41BF02E4-59D4-4006-AF96-C05B0D0EEA22}" name="couleur_1" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{1D1B1DBE-DA05-46F4-BA65-257985C82CB9}" name="score_1" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{C0BE1A05-5129-40A8-86C3-5B5052FF93BC}" name="score_2" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{859D60A2-6C69-45D2-8EF3-A58DF97DBC38}" name="couleur_2" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{2D02D19C-6174-4ACC-9EE3-74CAE6D8C11F}" name="joueur_2" dataDxfId="10"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3689F1AD-1BC0-4D5E-931C-5D5C9BFF293E}" name="Tableau13" displayName="Tableau13" ref="A1:H17" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:H17" xr:uid="{1FEF8CB5-F46E-43DE-981B-DE10EB7B0593}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{09A772A6-7CB9-48A0-892D-71FE6AF4CD86}" name="tour" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{3F0DAE02-7F7B-4C0F-9CB9-8220E03E9461}" name="match" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{BAE06CC9-48A4-4861-B83E-080730FD786C}" name="joueur_1" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{39B91494-18B6-451C-97B8-6FD72CB85619}" name="couleur_1" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{77626371-A1B6-4B83-8128-5D6CE115BF40}" name="score_1" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{3B9195C6-EB8B-4BA6-8F7B-596510A771D1}" name="score_2" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{C9E5E687-5273-47CA-B6DD-B4782D75B79A}" name="couleur_2" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{A1E2CD64-53C8-4C9A-B880-304BF16170A3}" name="joueur_2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -610,8 +919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FEF8CB5-F46E-43DE-981B-DE10EB7B0593}">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B9"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1082,7 +1391,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1279,4 +1588,914 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8DCFF8C-E59A-4BDE-A590-75B33EACBB1A}">
+  <dimension ref="A1:M17"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3">
+        <v>1</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0</v>
+      </c>
+      <c r="F13" s="3">
+        <v>1</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0</v>
+      </c>
+      <c r="F15" s="3">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0</v>
+      </c>
+      <c r="F16" s="3">
+        <v>1</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="3">
+        <v>1</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A36F5B85-9EA1-48A8-A937-7FF3B3DC85E3}">
+  <dimension ref="A1:M10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="M1" s="18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="13">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6">
+        <f>C2</f>
+        <v>1</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="5">
+        <v>1</v>
+      </c>
+      <c r="G2" s="6">
+        <f>F2+D2</f>
+        <v>2</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="J2" s="6">
+        <f>I2+G2</f>
+        <v>2.5</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="5">
+        <v>1</v>
+      </c>
+      <c r="M2" s="6">
+        <f>L2+J2</f>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="14">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="8">
+        <v>1</v>
+      </c>
+      <c r="D3" s="9">
+        <f t="shared" ref="D3:D9" si="0">C3</f>
+        <v>1</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="8">
+        <v>0</v>
+      </c>
+      <c r="G3" s="9">
+        <f>F3+D3</f>
+        <v>1</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="J3" s="9">
+        <f>I3+G5</f>
+        <v>2</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" s="8">
+        <v>0</v>
+      </c>
+      <c r="M3" s="9">
+        <f>L3+J4</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="14">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="D4" s="9">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="8">
+        <v>0</v>
+      </c>
+      <c r="G4" s="9">
+        <f>F4+D9</f>
+        <v>1</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="8">
+        <v>1</v>
+      </c>
+      <c r="J4" s="9">
+        <f>I4+G3</f>
+        <v>2</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="8">
+        <v>1</v>
+      </c>
+      <c r="M4" s="9">
+        <f>L4+J3</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="14">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="8">
+        <v>0</v>
+      </c>
+      <c r="D5" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="8">
+        <v>1</v>
+      </c>
+      <c r="G5" s="9">
+        <f>F5+D4</f>
+        <v>1.5</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="8">
+        <v>0</v>
+      </c>
+      <c r="J5" s="9">
+        <f>I5+G7</f>
+        <v>1</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="L5" s="8">
+        <v>0</v>
+      </c>
+      <c r="M5" s="9">
+        <f>L5+J7</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="14">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="8">
+        <v>0</v>
+      </c>
+      <c r="D6" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="20">
+        <v>0</v>
+      </c>
+      <c r="G6" s="9">
+        <f>F6+D8</f>
+        <v>0.5</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="20">
+        <v>0</v>
+      </c>
+      <c r="J6" s="9">
+        <f>I6+G4</f>
+        <v>1</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="L6" s="8">
+        <v>0</v>
+      </c>
+      <c r="M6" s="9">
+        <f>L6+J9</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="14">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0</v>
+      </c>
+      <c r="D7" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="20">
+        <v>1</v>
+      </c>
+      <c r="G7" s="9">
+        <f>F7+D5</f>
+        <v>1</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I7" s="20">
+        <v>1</v>
+      </c>
+      <c r="J7" s="9">
+        <f>I7+G8</f>
+        <v>1.5</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="L7" s="8">
+        <v>1</v>
+      </c>
+      <c r="M7" s="9">
+        <f>L7+J5</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="14">
+        <v>7</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="9">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="G8" s="9">
+        <f>F8+D6</f>
+        <v>0.5</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="20">
+        <v>0</v>
+      </c>
+      <c r="J8" s="9">
+        <f>I8+G9</f>
+        <v>0.5</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="L8" s="8">
+        <v>1</v>
+      </c>
+      <c r="M8" s="9">
+        <f>L8+J6</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="15">
+        <v>8</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="11">
+        <v>1</v>
+      </c>
+      <c r="D9" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="G9" s="12">
+        <f>F9+D7</f>
+        <v>0.5</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="I9" s="11">
+        <v>1</v>
+      </c>
+      <c r="J9" s="12">
+        <f>I9+G6</f>
+        <v>1.5</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="L9" s="11">
+        <v>0</v>
+      </c>
+      <c r="M9" s="12">
+        <f>L9+J8</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D10" s="21">
+        <f>SUM(D2:D9)</f>
+        <v>4</v>
+      </c>
+      <c r="G10" s="21">
+        <f>SUM(G2:G9)</f>
+        <v>8</v>
+      </c>
+      <c r="J10" s="21">
+        <f>SUM(J2:J9)</f>
+        <v>12</v>
+      </c>
+      <c r="M10" s="21">
+        <f>SUM(M2:M9)</f>
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>